<commit_message>
Feature/thfhjs fix bug (#1021)
* Convert int type to double

* Import  textStyle

* Shield the 'TAB' key and modify the default drawing

* change config file

* change Config file

* Datagrid Cell ficusable set False

Co-authored-by: THAPE\tiankaihe <1204973192@qq.com>
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/LoadCalculationConfig/房间功能映射表.xlsx
+++ b/AutoLoader/Contents/Support/LoadCalculationConfig/房间功能映射表.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AI研究中心\暖通调研\按指标计算负荷\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\AutoLoader\Contents\Support\LoadCalculationConfig\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1393,7 +1393,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>房间功能标签</t>
+    <t>暖通房间功能标签</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1777,7 +1777,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J303" sqref="J303"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1787,7 +1787,7 @@
     <col min="3" max="3" width="9.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.75" style="1" customWidth="1"/>
     <col min="5" max="5" width="21.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.25" style="3" customWidth="1"/>
     <col min="7" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>

</xml_diff>